<commit_message>
docs: requirement list, use case description, use case diagram 수정 - 자전거 상세 정보 조회, 자전거 리스트 조회 use case 분리
</commit_message>
<xml_diff>
--- a/최준서/Requirement List - 최준서(최종).xlsx
+++ b/최준서/Requirement List - 최준서(최종).xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>No.</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>관리자는 원하는 경우, 자전거 대여 정보(대여소 이름, 위치, 자전거 ID, 제품명, 유형)를 지역별 기준으로 정렬해서 조회할 수 있다.</t>
+  </si>
+  <si>
+    <t>관리자는 자전거 리스트 조회 화면에서 원하는 자전거 항목을 선택해서 상세내용(자전거 ID, 자전거 제품명, 유형(일반/전기), 소속 대여소, 상태(사용 가능/수리 중))화면을 볼 수 있다.</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1030,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.500000"/>
@@ -1075,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>19</v>

</xml_diff>